<commit_message>
Submit class and module's practice
include some new material also
</commit_message>
<xml_diff>
--- a/Training Plan.xlsx
+++ b/Training Plan.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
     <t>Content</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -313,25 +313,6 @@
     </r>
   </si>
   <si>
-    <t>类与对象</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>第三章 类与对象
-2.第七章 方法</t>
-    </r>
-  </si>
-  <si>
     <r>
       <t>1.</t>
     </r>
@@ -695,7 +676,27 @@
     <t>2015.02.10 9:00</t>
   </si>
   <si>
-    <t>2015.02.11 18:00</t>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>第三章 类与对象
+2.第七章 方法
+3.第八章 模块</t>
+    </r>
+  </si>
+  <si>
+    <t>2015.02.12 18:00</t>
+  </si>
+  <si>
+    <t>类与对象 方法 模块</t>
   </si>
 </sst>
 </file>
@@ -1295,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B6" sqref="A2:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1316,7 +1317,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1354,7 +1355,7 @@
     </row>
     <row r="2" spans="1:12" s="11" customFormat="1" ht="109" customHeight="1">
       <c r="A2" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="9">
         <v>0</v>
@@ -1378,16 +1379,16 @@
         <v>21</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="84">
@@ -1414,16 +1415,16 @@
         <v>21</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="L3" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="98">
@@ -1450,13 +1451,13 @@
         <v>27</v>
       </c>
       <c r="I4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="L4" s="1"/>
     </row>
@@ -1484,16 +1485,16 @@
         <v>33</v>
       </c>
       <c r="I5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="84">
@@ -1502,30 +1503,32 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="H6" s="13" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="I6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="84">
@@ -1534,28 +1537,28 @@
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>33</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1566,162 +1569,162 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="J8" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="42">
       <c r="A9" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="13" t="s">
+      <c r="I9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="J9" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="126">
       <c r="A10" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="H10" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="J10" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="77" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" s="1">
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="H11" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="56">
       <c r="A12" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>86</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1847,7 +1850,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="7"/>

</xml_diff>

<commit_message>
File Operations and Exception handling
Upload practice and update respective training plan
</commit_message>
<xml_diff>
--- a/Training Plan.xlsx
+++ b/Training Plan.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
   <si>
     <t>Content</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -175,9 +175,6 @@
     <t>Recommand Time</t>
   </si>
   <si>
-    <t>4 hours</t>
-  </si>
-  <si>
     <r>
       <t>1.</t>
     </r>
@@ -353,22 +350,6 @@
     <t>ruby 文件操作 和异常处理</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>第九章 异常
-2.第十章 基本I/O操作</t>
-    </r>
-  </si>
-  <si>
     <t>熟悉基本的IO操作Api以及异常处理方法</t>
   </si>
   <si>
@@ -384,27 +365,6 @@
         <charset val="134"/>
       </rPr>
       <t>实现一个文件操作类包含异常处理</t>
-    </r>
-  </si>
-  <si>
-    <t>2014.11.27 9:00</t>
-  </si>
-  <si>
-    <t>2014.11.27 18:00</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">practiceContent </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>中文件操作类需要能够新建文件 删除文件 读取文件内容，修改文件内容 需处理所有异常情况</t>
     </r>
   </si>
   <si>
@@ -463,12 +423,6 @@
       <t>安装rails的gems
 3.安装mysql数据库</t>
     </r>
-  </si>
-  <si>
-    <t>2014.11.28 9:00</t>
-  </si>
-  <si>
-    <t>2014.12.2 18:00</t>
   </si>
   <si>
     <t>Part</t>
@@ -697,6 +651,56 @@
   </si>
   <si>
     <t>类与对象 方法 模块</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>2015.02.13 9:00</t>
+  </si>
+  <si>
+    <t>2015.02.15 9:00</t>
+  </si>
+  <si>
+    <t>2015.02.17 18:00</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>第九章 异常
+2.第十一章 基本I/O操作</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PracticeContent </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中文件操作类需要能够
+1. 新建文件 
+2. 删除文件 
+3. 读取文件内容
+4. 修改文件内容 (需处理所有异常情况)</t>
+    </r>
+  </si>
+  <si>
+    <t>2015.02.13 18:00</t>
   </si>
 </sst>
 </file>
@@ -1296,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1317,7 +1321,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1355,7 +1359,7 @@
     </row>
     <row r="2" spans="1:12" s="11" customFormat="1" ht="109" customHeight="1">
       <c r="A2" s="17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B2" s="9">
         <v>0</v>
@@ -1376,19 +1380,19 @@
         <v>18</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="84">
@@ -1400,7 +1404,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
@@ -1412,19 +1416,19 @@
         <v>14</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="98">
@@ -1433,31 +1437,31 @@
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>27</v>
-      </c>
       <c r="I4" s="6" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="L4" s="1"/>
     </row>
@@ -1467,34 +1471,34 @@
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>33</v>
-      </c>
       <c r="I5" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="84">
@@ -1503,64 +1507,66 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="H6" s="13" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="84">
+    <row r="7" spans="1:12" ht="98">
       <c r="A7" s="18"/>
       <c r="B7" s="1">
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="1"/>
+        <v>103</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="70">
@@ -1569,162 +1575,162 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="42">
       <c r="A9" s="15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="J9" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="126">
       <c r="A10" s="15" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="77" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1">
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="56">
       <c r="A12" s="16" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1">
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="13" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1850,7 +1856,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="13" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="7"/>

</xml_diff>